<commit_message>
Updating table with results
</commit_message>
<xml_diff>
--- a/analysis/UFL/QLearningResults.xlsx
+++ b/analysis/UFL/QLearningResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\GrADyS\gradys-simulations\analysis\UFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732C4AE7-6356-4508-B9EF-D548DD155300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408092A2-CF00-4F6B-89D5-58A6A237E4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A891B27A-30F3-442C-87AE-923DAA3F8896}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Algorithm</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>2566c580d09b15b3611d29cbc08e798b9c9e07eb</t>
+  </si>
+  <si>
+    <t>Weighted average granular</t>
+  </si>
+  <si>
+    <t>5563bdff6251aa0ee740abc60fc275a0a5b92abf</t>
   </si>
 </sst>
 </file>
@@ -167,10 +173,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,7 +934,262 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CF64A1B-C520-38AE-0B52-ABAABCC6424C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="781050" cy="514350"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1040" name="Object 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1040"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC6764AD-4BB1-404D-90F3-DA4C6275A4C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="781050" cy="514350"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1041" name="Object 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1041"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77BD4241-98A7-483F-A0F3-256C686C1E97}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="781050" cy="514350"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="Object 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{481ED733-E9D3-4760-96A9-490804287A98}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="781050" cy="514350"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1047" name="Object 23" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1047"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{353171D3-0861-4102-9BD8-913501901821}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>781050</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1051" name="Object 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAF6BFED-9F63-E398-0114-5B65B77945AC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1275,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7F4EB0-E000-4546-BE0A-55C372F44514}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,11 +1575,11 @@
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1424,7 +1685,7 @@
       <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>44932</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -1435,25 +1696,42 @@
       <c r="H8" s="6"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7">
+        <v>44932</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7">
+        <v>44934</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="1"/>
     </row>
   </sheetData>
@@ -1815,6 +2093,131 @@
         <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1039" r:id="rId23"/>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1040" r:id="rId24">
+          <objectPr defaultSize="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>790575</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1040" r:id="rId24"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1041" r:id="rId25">
+          <objectPr defaultSize="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>781050</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1041" r:id="rId25"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1042" r:id="rId26">
+          <objectPr defaultSize="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>781050</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1042" r:id="rId26"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1047" r:id="rId27">
+          <objectPr defaultSize="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>790575</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1047" r:id="rId27"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1051" r:id="rId28">
+          <objectPr defaultSize="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>781050</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Objeto de Shell de Gerenciador" shapeId="1051" r:id="rId28"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>
</xml_diff>